<commit_message>
On-page audit in progress
</commit_message>
<xml_diff>
--- a/Audit-SEO-La-Chouette-Agence.xlsx
+++ b/Audit-SEO-La-Chouette-Agence.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericduprey/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericduprey/Desktop/My Htmls/10-La-Chouette-Agence/Starting website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36BF522-5702-C24C-8635-770BB426A1B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9BE9D6-A3F1-2441-8C25-033FE35BE0E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
   <si>
     <t>Catégorie</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>41_44 51_54</t>
-  </si>
-  <si>
-    <t>55_66</t>
   </si>
   <si>
     <t>image/png</t>
@@ -170,9 +167,6 @@
   </si>
   <si>
     <t>&lt;link rel="shortcut icon" type="image/png" href="favicon.jpg"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" type="text/css" href="./css/bootstrap.min.css" /&gt;</t>
   </si>
   <si>
     <t>&lt;link rel="stylesheet" type="text/css" href="./css/et-line.min.css" /&gt;</t>
@@ -279,17 +273,76 @@
     <t>img src="img/la-chouette-agence.png"</t>
   </si>
   <si>
-    <t>&lt;button id="nav-toggle" type="button" class="ui-navbar-toggle navbar-toggle" data-toggle="collapse" data-target=".navbar-1" data-target=".navbar-1" &gt;&lt;span class="sr-only"&gt;Toggle navigation&lt;/span
-                &gt;&lt;span class="icon-bar"&gt;&lt;/span&gt;&lt;span class="icon-bar"&gt;&lt;/span
-                &gt;&lt;span class="icon-bar"&gt;&lt;/span&gt;
-              &lt;/button&gt;</t>
+    <t>No description text</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" type="text/css" href="./css/et-line.css" /&gt;</t>
+  </si>
+  <si>
+    <t>Only : et-icon-browser, et-icon-presentation, et-icon-edit use in et-inline.css</t>
+  </si>
+  <si>
+    <t>Long tail keywords for begining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text that attracts with the main keywords </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO </t>
+  </si>
+  <si>
+    <t>Size and version image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove what is unnecessary </t>
+  </si>
+  <si>
+    <t>Minimize &amp; compress but remove if unused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define a title that contains keywords </t>
+  </si>
+  <si>
+    <t>Follow evolution</t>
+  </si>
+  <si>
+    <r>
+      <t>prioritize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color rgb="FF000000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Make a respectful code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color rgb="FF000000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>UX &amp; UI is important</t>
+  </si>
+  <si>
+    <t>Keyword in alt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,8 +394,13 @@
       <color theme="4"/>
       <name val="Menlo Regular"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +411,78 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -375,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +544,63 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,17 +817,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1006"/>
+  <dimension ref="A1:AA1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="94.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="62.28515625" customWidth="1"/>
     <col min="5" max="5" width="39" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" customWidth="1"/>
@@ -706,21 +893,21 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="A3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="17">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
@@ -730,25 +917,33 @@
         <v>21</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="E4" s="25" t="s">
+        <v>73</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="8">
+      <c r="A5" s="16"/>
+      <c r="B5" s="21">
         <v>9</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
+      <c r="C5" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1">
       <c r="A6" s="3"/>
@@ -765,322 +960,379 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:27" ht="17" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7">
+      <c r="A7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17">
         <v>14</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="E8" s="5"/>
+      <c r="C7" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:27" ht="17" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="7">
+        <v>19</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>77</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="12"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
+      <c r="A9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="17">
+        <v>21</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="29" t="s">
+        <v>78</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="7">
-        <v>22</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="A11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="17">
+        <v>23</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:27" ht="18" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <v>24</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7">
-        <v>23</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="29" t="s">
+        <v>78</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:27" ht="18" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="7">
-        <v>24</v>
-      </c>
-      <c r="C13" s="11" t="s">
+    <row r="13" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A13" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="17">
+        <v>25</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="7">
+        <v>27</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="7">
-        <v>25</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>79</v>
+      </c>
       <c r="F14" s="4"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="7">
-        <v>27</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
+      <c r="A15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>82</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="1:7" ht="58" customHeight="1">
+      <c r="A17" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" ht="21" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="58" customHeight="1">
-      <c r="A18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>82</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="21" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>71</v>
+    <row r="19" spans="1:7" ht="68" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7">
+        <v>119</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="117" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="68" customHeight="1">
+    <row r="20" spans="1:7" ht="69" customHeight="1">
+      <c r="A20" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="17">
+        <v>168</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="1:7" ht="77" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="7">
-        <v>119</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>27</v>
+        <v>199</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>83</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="69" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="7">
-        <v>168</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="77" customHeight="1">
+    <row r="22" spans="1:7" ht="76" customHeight="1">
+      <c r="A22" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="17">
+        <v>217</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="1:7" ht="105" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="7">
-        <v>199</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>30</v>
+        <v>372</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>82</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="76" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="7">
-        <v>217</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="105" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A24" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
-      <c r="B25" s="7">
-        <v>372</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="5" t="s">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="10"/>
       <c r="D27" s="3"/>
@@ -1088,202 +1340,232 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="1" t="s">
+    <row r="28" spans="1:7" ht="20" customHeight="1">
+      <c r="A28" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="17">
         <v>5</v>
       </c>
+      <c r="C28" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="B29" s="7">
+        <v>6</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="E29" s="26" t="s">
+        <v>74</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" ht="20" customHeight="1">
-      <c r="A30" s="3"/>
-      <c r="B30" s="7">
-        <v>5</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A31" s="3"/>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A30" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="17">
+        <v>7</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+    </row>
+    <row r="31" spans="1:7" ht="18" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="B31" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>76</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A32" s="3"/>
+      <c r="A32" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="B32" s="7">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>78</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A33" s="3"/>
-      <c r="B33" s="7">
-        <v>8</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="7">
-        <v>13</v>
+    <row r="33" spans="1:7" ht="96" customHeight="1">
+      <c r="A33" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" ht="65" customHeight="1">
+      <c r="A34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>80</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="7">
-        <v>16</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" ht="96" customHeight="1">
-      <c r="A36" s="3"/>
+    <row r="35" spans="1:7" ht="65" customHeight="1">
+      <c r="A35" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="21">
+        <v>41</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="1:7" ht="118" customHeight="1">
+      <c r="A36" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="B36" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>83</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="65" customHeight="1">
-      <c r="A37" s="3"/>
-      <c r="B37" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" ht="65" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="8">
-        <v>41</v>
+    <row r="37" spans="1:7" ht="123" customHeight="1">
+      <c r="A37" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="1:7" ht="117" customHeight="1">
+      <c r="A38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>83</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="118" customHeight="1">
-      <c r="A39" s="3"/>
-      <c r="B39" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>51</v>
-      </c>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A39" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="123" customHeight="1">
+    <row r="40" spans="1:7" ht="15.75" customHeight="1">
       <c r="A40" s="3"/>
-      <c r="B40" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" ht="117" customHeight="1">
+    <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="A41" s="3"/>
-      <c r="B41" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -1516,8 +1798,6 @@
     <row r="67" spans="1:7" ht="15.75" customHeight="1">
       <c r="A67" s="3"/>
       <c r="B67" s="7"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -1525,8 +1805,6 @@
     <row r="68" spans="1:7" ht="15.75" customHeight="1">
       <c r="A68" s="3"/>
       <c r="B68" s="7"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -1534,38 +1812,24 @@
     <row r="69" spans="1:7" ht="15.75" customHeight="1">
       <c r="A69" s="3"/>
       <c r="B69" s="7"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A70" s="3"/>
       <c r="B70" s="7"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A71" s="3"/>
       <c r="B71" s="7"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A72" s="3"/>
       <c r="B72" s="7"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1">
       <c r="B73" s="7"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1">
       <c r="B74" s="7"/>
@@ -1621,15 +1885,9 @@
     <row r="91" spans="2:2" ht="15.75" customHeight="1">
       <c r="B91" s="7"/>
     </row>
-    <row r="92" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B92" s="7"/>
-    </row>
-    <row r="93" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B93" s="7"/>
-    </row>
-    <row r="94" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B94" s="7"/>
-    </row>
+    <row r="92" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="93" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="94" spans="2:2" ht="15.75" customHeight="1"/>
     <row r="95" spans="2:2" ht="15.75" customHeight="1"/>
     <row r="96" spans="2:2" ht="15.75" customHeight="1"/>
     <row r="97" ht="15.75" customHeight="1"/>
@@ -2539,9 +2797,6 @@
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
     <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
-    <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>